<commit_message>
hyperparameter tunning plot codes
</commit_message>
<xml_diff>
--- a/Parameter_Testing_Ecoli.xlsx
+++ b/Parameter_Testing_Ecoli.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trisha/Programming/CompGenome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JHU\Fall2022\601.447Computational Genomics_Sequences\project\set-sketch-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5292BA52-4F01-8842-B061-F596E6906530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5810A5-D890-4627-98A1-EF0240C7FE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="3360" windowWidth="17280" windowHeight="16940" xr2:uid="{E1E10F89-1D6B-654B-81C6-191CBC164FD7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1E10F89-1D6B-654B-81C6-191CBC164FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="k" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="q" sheetId="5" r:id="rId4"/>
     <sheet name="a" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -424,15 +424,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67C0E4D-53AE-754B-B2E1-AA9524566E28}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I4" sqref="I4:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4</v>
       </c>
@@ -464,7 +464,7 @@
         <v>9.9000000000000199E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>8</v>
       </c>
@@ -472,15 +472,21 @@
         <v>9.5524399999999995E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>12</v>
       </c>
       <c r="B4">
         <v>0.167299</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>16</v>
       </c>
@@ -488,7 +494,7 @@
         <v>0.24288399999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>20</v>
       </c>
@@ -496,7 +502,7 @@
         <v>0.19549900000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>24</v>
       </c>
@@ -504,7 +510,7 @@
         <v>0.16291600000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>28</v>
       </c>
@@ -512,20 +518,12 @@
         <v>0.13964199999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>31</v>
       </c>
       <c r="B9">
         <v>0.12612799999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -541,9 +539,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -551,7 +549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5</v>
       </c>
@@ -559,7 +557,7 @@
         <v>0.12357600000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>15</v>
       </c>
@@ -567,7 +565,7 @@
         <v>9.7186300000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>25</v>
       </c>
@@ -588,9 +586,9 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -598,7 +596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.01</v>
       </c>
@@ -606,7 +604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -614,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.1499999999999999</v>
       </c>
@@ -622,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.18</v>
       </c>
@@ -630,7 +628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1.2</v>
       </c>
@@ -638,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1.22</v>
       </c>
@@ -646,7 +644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1.25</v>
       </c>
@@ -654,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1.28</v>
       </c>
@@ -662,7 +660,7 @@
         <v>1.49187E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1.33</v>
       </c>
@@ -670,7 +668,7 @@
         <v>7.58157E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1.4</v>
       </c>
@@ -678,7 +676,7 @@
         <v>9.3731700000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1.5</v>
       </c>
@@ -686,7 +684,7 @@
         <v>9.4788999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1.75</v>
       </c>
@@ -694,7 +692,7 @@
         <v>9.5532900000000004E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1.9</v>
       </c>
@@ -702,7 +700,7 @@
         <v>9.1822500000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1.95</v>
       </c>
@@ -720,12 +718,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B11" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -733,7 +731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -741,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>10</v>
       </c>
@@ -749,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>20</v>
       </c>
@@ -757,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>30</v>
       </c>
@@ -765,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>40</v>
       </c>
@@ -773,7 +771,7 @@
         <v>2.05246E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>60</v>
       </c>
@@ -781,7 +779,7 @@
         <v>9.4788999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>80</v>
       </c>
@@ -789,7 +787,7 @@
         <v>9.4788999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>90</v>
       </c>
@@ -797,7 +795,7 @@
         <v>9.4788999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>100</v>
       </c>
@@ -805,7 +803,7 @@
         <v>9.4788999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>110</v>
       </c>
@@ -826,9 +824,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -836,7 +834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -844,7 +842,7 @@
         <v>9.4424800000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>10</v>
       </c>
@@ -852,7 +850,7 @@
         <v>9.4158699999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>20</v>
       </c>
@@ -860,7 +858,7 @@
         <v>9.4788999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>30</v>
       </c>
@@ -868,7 +866,7 @@
         <v>9.4788999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>40</v>
       </c>
@@ -876,7 +874,7 @@
         <v>9.4693799999999995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>60</v>
       </c>

</xml_diff>